<commit_message>
Update strategy. Remove debugging files from Git tracking.
</commit_message>
<xml_diff>
--- a/strategy/2024-01-22.xlsx
+++ b/strategy/2024-01-22.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -711,7 +711,7 @@
         <v>45313.4583217593</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>54.6</v>
+        <v>51.6</v>
       </c>
       <c r="H13" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -738,7 +738,7 @@
         <v>45313.4999884259</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>54.6</v>
+        <v>51.6</v>
       </c>
       <c r="H14" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -765,7 +765,7 @@
         <v>45313.5416550926</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>54.6</v>
+        <v>53.6</v>
       </c>
       <c r="H15" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -792,7 +792,7 @@
         <v>45313.5833217593</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>54.6</v>
+        <v>51.6</v>
       </c>
       <c r="H16" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -819,7 +819,7 @@
         <v>45313.6249884259</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>54.6</v>
+        <v>51.6</v>
       </c>
       <c r="H17" s="1" t="n">
         <f aca="false">$H$3</f>

</xml_diff>